<commit_message>
Added changes to gui
</commit_message>
<xml_diff>
--- a/MyApplication_3/TouchGFX/assets/texts/texts.xlsx
+++ b/MyApplication_3/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1532" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1587" uniqueCount="88">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1645,7 +1645,7 @@
         <v>43</v>
       </c>
       <c r="D7">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E7">
         <v>4</v>

</xml_diff>